<commit_message>
IITM Stats1 Week2 mini project Frequency Table using Excel completed
</commit_message>
<xml_diff>
--- a/IIT_Madras-Excel_Projects-Statistics_Foundation_Level-Data_Science-BS_Degree/DataSets/IITM - Stats 1 - Hospital Dataset Copy.xlsx
+++ b/IIT_Madras-Excel_Projects-Statistics_Foundation_Level-Data_Science-BS_Degree/DataSets/IITM - Stats 1 - Hospital Dataset Copy.xlsx
@@ -1,18 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Shubham-Data-Analytics\Data-Analytics-GitHub\IIT_Madras-Excel_Projects-Statistics_Foundation_Level-Data_Science-BS_Degree\DataSets\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBD19785-AE03-4FD1-BE12-C03D2D2BE848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Pivot Table 1 Gender" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Pivot Table 2 Blood Group" sheetId="3" r:id="rId6"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Pivot Table 1 Gender" sheetId="2" r:id="rId2"/>
+    <sheet name="Pivot Table 2 Blood Group" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId7"/>
-    <pivotCache cacheId="1" r:id="rId8"/>
+    <pivotCache cacheId="5" r:id="rId4"/>
+    <pivotCache cacheId="9" r:id="rId5"/>
   </pivotCaches>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -181,32 +201,32 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="h:mm:ss am/pm"/>
-    <numFmt numFmtId="165" formatCode="M/d/yyyy"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Roboto"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
@@ -217,7 +237,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -232,8 +252,14 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
-    <border/>
+  <borders count="8">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -247,94 +273,144 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF999999"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF999999"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+  <cellXfs count="18">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="19" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="165" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="19" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" pivotButton="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" invalid="1" refreshOnLoad="1">
-  <cacheSource type="worksheet">
-    <worksheetSource ref="E1:E31" sheet="Sheet1"/>
-  </cacheSource>
-  <cacheFields>
-    <cacheField name="Gender" numFmtId="0">
-      <sharedItems>
-        <s v="M"/>
-        <s v="F"/>
-      </sharedItems>
-    </cacheField>
-  </cacheFields>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" invalid="1" refreshOnLoad="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="shubham gupta" refreshedDate="45421.876485532404" refreshedVersion="8" recordCount="30" xr:uid="{00000000-000A-0000-FFFF-FFFF01000000}">
   <cacheSource type="worksheet">
     <worksheetSource ref="G1:G31" sheet="Sheet1"/>
   </cacheSource>
-  <cacheFields>
+  <cacheFields count="1">
     <cacheField name="Blood Group" numFmtId="0">
-      <sharedItems>
+      <sharedItems count="8">
         <s v="O+"/>
         <s v="A-"/>
         <s v="O-"/>
@@ -346,36 +422,272 @@
       </sharedItems>
     </cacheField>
   </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="shubham gupta" refreshedDate="45421.876485763889" refreshedVersion="8" recordCount="30" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="E1:E31" sheet="Sheet1"/>
+  </cacheSource>
+  <cacheFields count="1">
+    <cacheField name="Gender" numFmtId="0">
+      <sharedItems count="2">
+        <s v="M"/>
+        <s v="F"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="30">
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="6"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="5"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="7"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="4"/>
+  </r>
+  <r>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="30">
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Pivot Table 1 Gender" cacheId="0" dataCaption="" compact="0" compactData="0">
-  <location ref="A1:B4" firstHeaderRow="0" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="Pivot Table 1 Gender" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="8" compact="0" compactData="0">
+  <location ref="A1:B4" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="1">
     <pivotField name="Gender" axis="axisRow" dataField="1" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
-      <items>
+      <items count="3">
         <item x="1"/>
         <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
   </pivotFields>
-  <rowFields>
+  <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <dataFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
     <dataField name="COUNTA of Gender" fld="0" subtotal="count" baseField="0"/>
   </dataFields>
+  <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
 </pivotTableDefinition>
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Pivot Table 2 Blood Group" cacheId="1" dataCaption="" compact="0" compactData="0">
-  <location ref="A1:B10" firstHeaderRow="0" firstDataRow="1" firstDataCol="0"/>
-  <pivotFields>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000001000000}" name="Pivot Table 2 Blood Group" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="8" compact="0" compactData="0">
+  <location ref="A1:B10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="1">
     <pivotField name="Blood Group" axis="axisRow" dataField="1" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
-      <items>
+      <items count="9">
         <item x="1"/>
         <item x="4"/>
         <item x="7"/>
@@ -388,17 +700,55 @@
       </items>
     </pivotField>
   </pivotFields>
-  <rowFields>
+  <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <dataFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
     <dataField name="COUNTA of Blood Group" fld="0" subtotal="count" baseField="0"/>
   </dataFields>
+  <pivotTableStyleInfo showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
 </pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -588,25 +938,28 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="19.5"/>
-    <col customWidth="1" min="8" max="8" width="19.38"/>
-    <col customWidth="1" min="9" max="9" width="19.5"/>
+    <col min="2" max="2" width="19.44140625" customWidth="1"/>
+    <col min="8" max="8" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -635,47 +988,47 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
-        <v>1.0</v>
+        <v>1</v>
       </c>
       <c r="B2" s="4">
-        <v>43864.0</v>
+        <v>43864</v>
       </c>
       <c r="C2" s="5">
         <v>0.3125</v>
       </c>
       <c r="D2" s="3">
-        <v>178.0</v>
+        <v>178</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F2" s="3">
-        <v>75.0</v>
+        <v>75</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>10</v>
       </c>
       <c r="H2" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>2.0</v>
+        <v>2</v>
       </c>
       <c r="B3" s="4">
-        <v>43864.0</v>
+        <v>43864</v>
       </c>
       <c r="C3" s="5">
-        <v>0.3333333333333333</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D3" s="3">
-        <v>150.0</v>
+        <v>150</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>12</v>
@@ -693,24 +1046,24 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>3.0</v>
+        <v>3</v>
       </c>
       <c r="B4" s="4">
-        <v>43864.0</v>
+        <v>43864</v>
       </c>
       <c r="C4" s="5">
-        <v>0.3416666666666667</v>
+        <v>0.34166666666666667</v>
       </c>
       <c r="D4" s="3">
-        <v>162.0</v>
+        <v>162</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F4" s="3">
-        <v>61.0</v>
+        <v>61</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>15</v>
@@ -722,24 +1075,24 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>4.0</v>
+        <v>4</v>
       </c>
       <c r="B5" s="4">
-        <v>43864.0</v>
+        <v>43864</v>
       </c>
       <c r="C5" s="5">
         <v>0.36944444444444446</v>
       </c>
       <c r="D5" s="3">
-        <v>145.0</v>
+        <v>145</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F5" s="3">
-        <v>65.0</v>
+        <v>65</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>17</v>
@@ -751,24 +1104,24 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>5.0</v>
+        <v>5</v>
       </c>
       <c r="B6" s="4">
-        <v>43864.0</v>
+        <v>43864</v>
       </c>
       <c r="C6" s="5">
         <v>0.375</v>
       </c>
       <c r="D6" s="3">
-        <v>153.0</v>
+        <v>153</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F6" s="3">
-        <v>72.0</v>
+        <v>72</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>19</v>
@@ -780,140 +1133,140 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>6.0</v>
+        <v>6</v>
       </c>
       <c r="B7" s="4">
-        <v>43864.0</v>
+        <v>43864</v>
       </c>
       <c r="C7" s="5">
-        <v>0.38125</v>
+        <v>0.38124999999999998</v>
       </c>
       <c r="D7" s="3">
-        <v>167.0</v>
+        <v>167</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F7" s="3">
-        <v>98.0</v>
+        <v>98</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>10</v>
       </c>
       <c r="H7" s="3">
-        <v>110.0</v>
+        <v>110</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
-        <v>7.0</v>
+        <v>7</v>
       </c>
       <c r="B8" s="4">
-        <v>43864.0</v>
+        <v>43864</v>
       </c>
       <c r="C8" s="5">
-        <v>0.4166666666666667</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="D8" s="3">
-        <v>175.0</v>
+        <v>175</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F8" s="3">
-        <v>69.0</v>
+        <v>69</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>22</v>
       </c>
       <c r="H8" s="3">
-        <v>94.0</v>
+        <v>94</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
-        <v>8.0</v>
+        <v>8</v>
       </c>
       <c r="B9" s="4">
-        <v>43864.0</v>
+        <v>43864</v>
       </c>
       <c r="C9" s="5">
         <v>0.4236111111111111</v>
       </c>
       <c r="D9" s="3">
-        <v>165.0</v>
+        <v>165</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F9" s="3">
-        <v>59.0</v>
+        <v>59</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H9" s="3">
-        <v>93.0</v>
+        <v>93</v>
       </c>
       <c r="I9" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
-        <v>9.0</v>
+        <v>9</v>
       </c>
       <c r="B10" s="4">
-        <v>43893.0</v>
+        <v>43893</v>
       </c>
       <c r="C10" s="5">
-        <v>0.3194444444444444</v>
+        <v>0.31944444444444442</v>
       </c>
       <c r="D10" s="3">
-        <v>169.0</v>
+        <v>169</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F10" s="3">
-        <v>65.0</v>
+        <v>65</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H10" s="3">
-        <v>96.0</v>
+        <v>96</v>
       </c>
       <c r="I10" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
-        <v>10.0</v>
+        <v>10</v>
       </c>
       <c r="B11" s="4">
-        <v>43893.0</v>
+        <v>43893</v>
       </c>
       <c r="C11" s="5">
-        <v>0.3326388888888889</v>
+        <v>0.33263888888888887</v>
       </c>
       <c r="D11" s="3">
-        <v>173.0</v>
+        <v>173</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F11" s="3">
-        <v>74.0</v>
+        <v>74</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>26</v>
@@ -925,24 +1278,24 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
-        <v>11.0</v>
+        <v>11</v>
       </c>
       <c r="B12" s="4">
-        <v>43893.0</v>
+        <v>43893</v>
       </c>
       <c r="C12" s="5">
         <v>0.33402777777777776</v>
       </c>
       <c r="D12" s="3">
-        <v>156.0</v>
+        <v>156</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F12" s="3">
-        <v>61.0</v>
+        <v>61</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>15</v>
@@ -954,24 +1307,24 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
-        <v>12.0</v>
+        <v>12</v>
       </c>
       <c r="B13" s="4">
-        <v>43893.0</v>
+        <v>43893</v>
       </c>
       <c r="C13" s="5">
         <v>0.34375</v>
       </c>
       <c r="D13" s="3">
-        <v>158.0</v>
+        <v>158</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F13" s="3">
-        <v>52.0</v>
+        <v>52</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>17</v>
@@ -983,53 +1336,53 @@
         <v>29</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
-        <v>13.0</v>
+        <v>13</v>
       </c>
       <c r="B14" s="4">
-        <v>43893.0</v>
+        <v>43893</v>
       </c>
       <c r="C14" s="5">
         <v>0.36180555555555555</v>
       </c>
       <c r="D14" s="3">
-        <v>183.0</v>
+        <v>183</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F14" s="3">
-        <v>82.0</v>
+        <v>82</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>30</v>
       </c>
       <c r="H14" s="3">
-        <v>102.0</v>
+        <v>102</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
-        <v>14.0</v>
+        <v>14</v>
       </c>
       <c r="B15" s="4">
-        <v>43893.0</v>
+        <v>43893</v>
       </c>
       <c r="C15" s="5">
         <v>0.375</v>
       </c>
       <c r="D15" s="3">
-        <v>167.0</v>
+        <v>167</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F15" s="3">
-        <v>71.0</v>
+        <v>71</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>22</v>
@@ -1041,24 +1394,24 @@
         <v>31</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
-        <v>15.0</v>
+        <v>15</v>
       </c>
       <c r="B16" s="4">
-        <v>43893.0</v>
+        <v>43893</v>
       </c>
       <c r="C16" s="5">
-        <v>0.3958333333333333</v>
+        <v>0.39583333333333331</v>
       </c>
       <c r="D16" s="3">
-        <v>169.0</v>
+        <v>169</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F16" s="3">
-        <v>63.0</v>
+        <v>63</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>19</v>
@@ -1070,24 +1423,24 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
-        <v>16.0</v>
+        <v>16</v>
       </c>
       <c r="B17" s="4">
-        <v>43924.0</v>
+        <v>43924</v>
       </c>
       <c r="C17" s="5">
-        <v>0.3055555555555556</v>
+        <v>0.30555555555555558</v>
       </c>
       <c r="D17" s="3">
-        <v>171.0</v>
+        <v>171</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F17" s="3">
-        <v>70.0</v>
+        <v>70</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>26</v>
@@ -1099,53 +1452,53 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>17.0</v>
+        <v>17</v>
       </c>
       <c r="B18" s="4">
-        <v>43924.0</v>
+        <v>43924</v>
       </c>
       <c r="C18" s="5">
         <v>0.35208333333333336</v>
       </c>
       <c r="D18" s="3">
-        <v>163.0</v>
+        <v>163</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F18" s="3">
-        <v>67.0</v>
+        <v>67</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>15</v>
       </c>
       <c r="H18" s="3">
-        <v>98.0</v>
+        <v>98</v>
       </c>
       <c r="I18" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
-        <v>18.0</v>
+        <v>18</v>
       </c>
       <c r="B19" s="4">
-        <v>43924.0</v>
+        <v>43924</v>
       </c>
       <c r="C19" s="5">
         <v>0.40625</v>
       </c>
       <c r="D19" s="3">
-        <v>155.0</v>
+        <v>155</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3">
-        <v>64.0</v>
+        <v>64</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>22</v>
@@ -1157,53 +1510,53 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
-        <v>19.0</v>
+        <v>19</v>
       </c>
       <c r="B20" s="4">
-        <v>43924.0</v>
+        <v>43924</v>
       </c>
       <c r="C20" s="5">
         <v>0.41388888888888886</v>
       </c>
       <c r="D20" s="3">
-        <v>150.0</v>
+        <v>150</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F20" s="3">
-        <v>55.0</v>
+        <v>55</v>
       </c>
       <c r="G20" s="3" t="s">
         <v>19</v>
       </c>
       <c r="H20" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="I20" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
-        <v>20.0</v>
+        <v>20</v>
       </c>
       <c r="B21" s="6">
-        <v>43924.0</v>
+        <v>43924</v>
       </c>
       <c r="C21" s="5">
         <v>0.36041666666666666</v>
       </c>
       <c r="D21" s="3">
-        <v>145.0</v>
+        <v>145</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F21" s="3">
-        <v>58.0</v>
+        <v>58</v>
       </c>
       <c r="G21" s="3" t="s">
         <v>30</v>
@@ -1215,82 +1568,82 @@
         <v>37</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
-        <v>21.0</v>
+        <v>21</v>
       </c>
       <c r="B22" s="6">
-        <v>43924.0</v>
+        <v>43924</v>
       </c>
       <c r="C22" s="5">
         <v>0.3298611111111111</v>
       </c>
       <c r="D22" s="3">
-        <v>174.0</v>
+        <v>174</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F22" s="3">
-        <v>74.0</v>
+        <v>74</v>
       </c>
       <c r="G22" s="3" t="s">
         <v>10</v>
       </c>
       <c r="H22" s="3">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="I22" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
-        <v>22.0</v>
+        <v>22</v>
       </c>
       <c r="B23" s="6">
-        <v>43924.0</v>
+        <v>43924</v>
       </c>
       <c r="C23" s="5">
         <v>0.42916666666666664</v>
       </c>
       <c r="D23" s="3">
-        <v>167.0</v>
+        <v>167</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F23" s="3">
-        <v>68.0</v>
+        <v>68</v>
       </c>
       <c r="G23" s="3" t="s">
         <v>17</v>
       </c>
       <c r="H23" s="3">
-        <v>101.0</v>
+        <v>101</v>
       </c>
       <c r="I23" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
-        <v>23.0</v>
+        <v>23</v>
       </c>
       <c r="B24" s="6">
-        <v>43924.0</v>
+        <v>43924</v>
       </c>
       <c r="C24" s="5">
-        <v>0.3590277777777778</v>
+        <v>0.35902777777777778</v>
       </c>
       <c r="D24" s="3">
-        <v>162.0</v>
+        <v>162</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F24" s="3">
-        <v>71.0</v>
+        <v>71</v>
       </c>
       <c r="G24" s="3" t="s">
         <v>19</v>
@@ -1302,53 +1655,53 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
-        <v>24.0</v>
+        <v>24</v>
       </c>
       <c r="B25" s="4">
-        <v>43954.0</v>
+        <v>43954</v>
       </c>
       <c r="C25" s="5">
         <v>0.31666666666666665</v>
       </c>
       <c r="D25" s="3">
-        <v>158.0</v>
+        <v>158</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F25" s="3">
-        <v>56.0</v>
+        <v>56</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>10</v>
       </c>
       <c r="H25" s="3">
-        <v>99.0</v>
+        <v>99</v>
       </c>
       <c r="I25" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>25.0</v>
+        <v>25</v>
       </c>
       <c r="B26" s="6">
-        <v>43954.0</v>
+        <v>43954</v>
       </c>
       <c r="C26" s="5">
-        <v>0.4479166666666667</v>
+        <v>0.44791666666666669</v>
       </c>
       <c r="D26" s="3">
-        <v>149.0</v>
+        <v>149</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F26" s="3">
-        <v>49.0</v>
+        <v>49</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>17</v>
@@ -1360,24 +1713,24 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
-        <v>26.0</v>
+        <v>26</v>
       </c>
       <c r="B27" s="6">
-        <v>43954.0</v>
+        <v>43954</v>
       </c>
       <c r="C27" s="5">
         <v>0.38263888888888886</v>
       </c>
       <c r="D27" s="3">
-        <v>175.0</v>
+        <v>175</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F27" s="3">
-        <v>76.0</v>
+        <v>76</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>30</v>
@@ -1389,24 +1742,24 @@
         <v>42</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
-        <v>27.0</v>
+        <v>27</v>
       </c>
       <c r="B28" s="6">
-        <v>43954.0</v>
+        <v>43954</v>
       </c>
       <c r="C28" s="5">
         <v>0.35208333333333336</v>
       </c>
       <c r="D28" s="3">
-        <v>157.0</v>
+        <v>157</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F28" s="3">
-        <v>63.0</v>
+        <v>63</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>13</v>
@@ -1418,24 +1771,24 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
-        <v>28.0</v>
+        <v>28</v>
       </c>
       <c r="B29" s="6">
-        <v>43954.0</v>
+        <v>43954</v>
       </c>
       <c r="C29" s="5">
         <v>0.36041666666666666</v>
       </c>
       <c r="D29" s="3">
-        <v>169.0</v>
+        <v>169</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F29" s="3">
-        <v>69.0</v>
+        <v>69</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>19</v>
@@ -1447,24 +1800,24 @@
         <v>18</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
-        <v>29.0</v>
+        <v>29</v>
       </c>
       <c r="B30" s="6">
-        <v>43954.0</v>
+        <v>43954</v>
       </c>
       <c r="C30" s="5">
         <v>0.39305555555555555</v>
       </c>
       <c r="D30" s="3">
-        <v>158.0</v>
+        <v>158</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>12</v>
       </c>
       <c r="F30" s="3">
-        <v>55.0</v>
+        <v>55</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>15</v>
@@ -1476,253 +1829,353 @@
         <v>44</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
-        <v>30.0</v>
+        <v>30</v>
       </c>
       <c r="B31" s="6">
-        <v>43954.0</v>
+        <v>43954</v>
       </c>
       <c r="C31" s="5">
-        <v>0.3729166666666667</v>
+        <v>0.37291666666666667</v>
       </c>
       <c r="D31" s="3">
-        <v>176.0</v>
+        <v>176</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>9</v>
       </c>
       <c r="F31" s="3">
-        <v>78.0</v>
+        <v>78</v>
       </c>
       <c r="G31" s="3" t="s">
         <v>10</v>
       </c>
       <c r="H31" s="3">
-        <v>100.0</v>
+        <v>100</v>
       </c>
       <c r="I31" s="3" t="s">
         <v>45</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="19.88"/>
+    <col min="3" max="3" width="19.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1"/>
-    <row r="2"/>
-    <row r="3"/>
-    <row r="4"/>
-    <row r="6">
-      <c r="A6" s="8" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="13">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="17">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="9">
-        <v>11.0</v>
-      </c>
-      <c r="C7" s="9">
-        <f t="shared" ref="C7:C9" si="1">B7/B$9</f>
-        <v>0.3666666667</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="9" t="s">
+      <c r="B7" s="7">
+        <v>11</v>
+      </c>
+      <c r="C7" s="7">
+        <f t="shared" ref="C7:C9" si="0">B7/B$9</f>
+        <v>0.36666666666666664</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="9">
-        <v>19.0</v>
-      </c>
-      <c r="C8" s="9">
-        <f t="shared" si="1"/>
-        <v>0.6333333333</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="9" t="s">
+      <c r="B8" s="7">
+        <v>19</v>
+      </c>
+      <c r="C8" s="7">
+        <f t="shared" si="0"/>
+        <v>0.6333333333333333</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="B9" s="9">
-        <v>30.0</v>
-      </c>
-      <c r="C9" s="9">
-        <f t="shared" si="1"/>
+      <c r="B9" s="7">
+        <v>30</v>
+      </c>
+      <c r="C9" s="7">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="14.38"/>
-    <col customWidth="1" min="3" max="3" width="20.0"/>
+    <col min="1" max="1" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1"/>
-    <row r="2"/>
-    <row r="3"/>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7"/>
-    <row r="8"/>
-    <row r="9"/>
-    <row r="10"/>
-    <row r="12">
-      <c r="A12" s="10" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="17">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="C12" s="9" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="13">
-      <c r="A13" s="12" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="12">
-        <v>2.0</v>
-      </c>
-      <c r="C13" s="13">
-        <f t="shared" ref="C13:C21" si="1">B13/B$21</f>
-        <v>0.06666666667</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="12" t="s">
+      <c r="B13" s="8">
+        <v>2</v>
+      </c>
+      <c r="C13" s="9">
+        <f t="shared" ref="C13:C21" si="0">B13/B$21</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="12">
-        <v>6.0</v>
-      </c>
-      <c r="C14" s="13">
-        <f t="shared" si="1"/>
+      <c r="B14" s="8">
+        <v>6</v>
+      </c>
+      <c r="C14" s="9">
+        <f t="shared" si="0"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="15">
-      <c r="A15" s="12" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="12">
-        <v>3.0</v>
-      </c>
-      <c r="C15" s="13">
-        <f t="shared" si="1"/>
+      <c r="B15" s="8">
+        <v>3</v>
+      </c>
+      <c r="C15" s="9">
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" s="12" t="s">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B16" s="12">
-        <v>2.0</v>
-      </c>
-      <c r="C16" s="13">
-        <f t="shared" si="1"/>
-        <v>0.06666666667</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="12" t="s">
+      <c r="B16" s="8">
+        <v>2</v>
+      </c>
+      <c r="C16" s="9">
+        <f t="shared" si="0"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="12">
-        <v>3.0</v>
-      </c>
-      <c r="C17" s="13">
-        <f t="shared" si="1"/>
+      <c r="B17" s="8">
+        <v>3</v>
+      </c>
+      <c r="C17" s="9">
+        <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" s="12" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="12">
-        <v>4.0</v>
-      </c>
-      <c r="C18" s="13">
-        <f t="shared" si="1"/>
-        <v>0.1333333333</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="12" t="s">
+      <c r="B18" s="8">
+        <v>4</v>
+      </c>
+      <c r="C18" s="9">
+        <f t="shared" si="0"/>
+        <v>0.13333333333333333</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="12">
-        <v>5.0</v>
-      </c>
-      <c r="C19" s="13">
-        <f t="shared" si="1"/>
-        <v>0.1666666667</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="12" t="s">
+      <c r="B19" s="8">
+        <v>5</v>
+      </c>
+      <c r="C19" s="9">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B20" s="12">
-        <v>5.0</v>
-      </c>
-      <c r="C20" s="13">
-        <f t="shared" si="1"/>
-        <v>0.1666666667</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="12" t="s">
+      <c r="B20" s="8">
+        <v>5</v>
+      </c>
+      <c r="C20" s="9">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="12">
-        <v>30.0</v>
-      </c>
-      <c r="C21" s="13">
-        <f t="shared" si="1"/>
+      <c r="B21" s="8">
+        <v>30</v>
+      </c>
+      <c r="C21" s="9">
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId2"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>